<commit_message>
TX power level can be selected with J, K, L. Configured for CW (no fract div)
</commit_message>
<xml_diff>
--- a/Fractional divider test.xlsx
+++ b/Fractional divider test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="14">
   <si>
     <t xml:space="preserve">Xtal=</t>
   </si>
@@ -230,7 +230,7 @@
   <dimension ref="B9:N74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -240,7 +240,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="0" t="n">
-        <v>25000000</v>
+        <v>24999822</v>
       </c>
       <c r="J9" s="0" t="s">
         <v>0</v>
@@ -297,7 +297,7 @@
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">8192*(C14*C10*C11/C9-C12)</f>
-        <v>4299.03052800009</v>
+        <v>8613.57773955353</v>
       </c>
       <c r="M13" s="0" t="s">
         <v>4</v>
@@ -312,7 +312,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>7010100</v>
+        <v>7018300</v>
       </c>
       <c r="J14" s="0" t="s">
         <v>5</v>
@@ -345,9 +345,6 @@
       <c r="K17" s="0" t="n">
         <v>2033</v>
       </c>
-      <c r="M17" s="0" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="0" t="s">
@@ -355,7 +352,7 @@
       </c>
       <c r="C18" s="0" t="n">
         <f aca="false">(C17/8192+C12)*C9/C10/C11</f>
-        <v>7001879.69924812</v>
+        <v>7001829.84586466</v>
       </c>
       <c r="J18" s="0" t="s">
         <v>9</v>
@@ -371,7 +368,7 @@
       </c>
       <c r="C20" s="0" t="n">
         <f aca="false">C18-(C17+1+8192*C12)/0.52297728</f>
-        <v>-1.91212895512581</v>
+        <v>-51.7655124133453</v>
       </c>
       <c r="J20" s="0" t="s">
         <v>10</v>
@@ -387,7 +384,7 @@
       </c>
       <c r="C23" s="0" t="n">
         <f aca="false">((C17+1)/8192+C12)*C9/C10/C11</f>
-        <v>7001881.61137708</v>
+        <v>7001831.75798</v>
       </c>
       <c r="J23" s="0" t="s">
         <v>11</v>
@@ -403,7 +400,7 @@
       </c>
       <c r="C25" s="0" t="n">
         <f aca="false">C23-C18</f>
-        <v>1.91212895512581</v>
+        <v>1.91211534105241</v>
       </c>
       <c r="J25" s="0" t="s">
         <v>10</v>

</xml_diff>